<commit_message>
Update for Speed Quiz 2023-5-9
</commit_message>
<xml_diff>
--- a/scripts/QuizConfigHelper.xlsx
+++ b/scripts/QuizConfigHelper.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrej\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7265B84-383D-4B67-873B-2FD39419826A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5BC39A-1063-4EAA-A0B7-4F0461C426BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1A1E301B-5405-4BF5-94E3-74BAFB9EEE14}"/>
+    <workbookView xWindow="-28920" yWindow="-1995" windowWidth="29040" windowHeight="17640" xr2:uid="{1A1E301B-5405-4BF5-94E3-74BAFB9EEE14}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="2" r:id="rId1"/>
     <sheet name="2023-5-5" sheetId="1" r:id="rId2"/>
+    <sheet name="2023-5-9" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>0</t>
   </si>
@@ -93,7 +94,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -103,6 +104,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -119,17 +126,184 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="30">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -160,6 +334,170 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
         <color theme="0"/>
         <name val="Calibri"/>
         <family val="2"/>
@@ -202,114 +540,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -327,6 +557,114 @@
         <color auto="1"/>
         <name val="Calibri"/>
         <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
         <scheme val="none"/>
       </font>
     </dxf>
@@ -342,153 +680,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
+        <color theme="0"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -508,14 +700,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{95E507F7-1E07-427A-A363-C0FB487EC785}" name="Table13" displayName="Table13" ref="A1:E27" totalsRowCount="1" headerRowDxfId="0" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{95E507F7-1E07-427A-A363-C0FB487EC785}" name="Table13" displayName="Table13" ref="A1:E27" totalsRowCount="1" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="A1:E26" xr:uid="{C9AE075E-B9D0-44B1-A335-E02B884B531E}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{C69BBE94-502E-47D3-A9AA-F194F354155A}" name="0"/>
-    <tableColumn id="2" xr3:uid="{1FB0E793-A471-497D-88C4-949E9BFA0C8F}" name="1" dataDxfId="8" totalsRowDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{89F2C03D-ED22-4063-911D-E7373DEF9496}" name="2" dataDxfId="7" totalsRowDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{1FA3B4D5-8641-4F49-9616-E0366217905E}" name="3" dataDxfId="6" totalsRowDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{91B96506-156E-4C32-99E8-0DE63DDC8C37}" name="FULL" totalsRowFunction="custom" dataDxfId="9" totalsRowDxfId="2">
+    <tableColumn id="2" xr3:uid="{1FB0E793-A471-497D-88C4-949E9BFA0C8F}" name="1" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{89F2C03D-ED22-4063-911D-E7373DEF9496}" name="2" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{1FA3B4D5-8641-4F49-9616-E0366217905E}" name="3" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{91B96506-156E-4C32-99E8-0DE63DDC8C37}" name="FULL" totalsRowFunction="custom" dataDxfId="21" totalsRowDxfId="20">
       <calculatedColumnFormula>IF(Table13[[#This Row],[1]]&lt;&gt;"",Table13[[#This Row],[1]],IF(Table13[[#This Row],[2]]&lt;&gt;"",Table13[[#This Row],[2]],IF(Table13[[#This Row],[3]]&lt;&gt;"",Table13[[#This Row],[3]],"-")))</calculatedColumnFormula>
       <totalsRowFormula>"[0"&amp;","&amp;E2&amp;","&amp;E3&amp;","&amp;E4&amp;","&amp;E5&amp;","&amp;E6&amp;","&amp;E7&amp;","&amp;E8&amp;","&amp;E9&amp;","&amp;E10&amp;","&amp;E11&amp;","&amp;E12&amp;","&amp;E13&amp;","&amp;E14&amp;","&amp;E15&amp;","&amp;E16&amp;","&amp;E17&amp;","&amp;E18&amp;","&amp;E19&amp;","&amp;E20&amp;","&amp;E21&amp;","&amp;E22&amp;","&amp;E23&amp;","&amp;E24&amp;","&amp;E25&amp;","&amp;E26&amp;"]"</totalsRowFormula>
     </tableColumn>
@@ -525,15 +717,32 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C9AE075E-B9D0-44B1-A335-E02B884B531E}" name="Table1" displayName="Table1" ref="A1:E27" totalsRowCount="1" headerRowDxfId="1" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C9AE075E-B9D0-44B1-A335-E02B884B531E}" name="Table1" displayName="Table1" ref="A1:E27" totalsRowCount="1" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A1:E26" xr:uid="{C9AE075E-B9D0-44B1-A335-E02B884B531E}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{DCFB1B30-AA68-4524-AF80-5AFE18AC05BB}" name="0"/>
-    <tableColumn id="2" xr3:uid="{A90B6EEB-FC8B-4231-A5E2-A31293EDB551}" name="1" dataDxfId="18" totalsRowDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{585B8F47-B526-4C76-86B8-BE40EFC8C722}" name="2" dataDxfId="16" totalsRowDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{54B78388-3C67-4184-9ECE-F5B91C34B9B0}" name="3" dataDxfId="14" totalsRowDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{8EAC5146-454C-4D49-93CC-6E35149D5DE1}" name="FULL" totalsRowFunction="custom" dataDxfId="12" totalsRowDxfId="11">
+    <tableColumn id="2" xr3:uid="{A90B6EEB-FC8B-4231-A5E2-A31293EDB551}" name="1" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{585B8F47-B526-4C76-86B8-BE40EFC8C722}" name="2" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{54B78388-3C67-4184-9ECE-F5B91C34B9B0}" name="3" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{8EAC5146-454C-4D49-93CC-6E35149D5DE1}" name="FULL" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="10">
       <calculatedColumnFormula>IF(Table1[[#This Row],[1]]&lt;&gt;"",Table1[[#This Row],[1]],IF(Table1[[#This Row],[2]]&lt;&gt;"",Table1[[#This Row],[2]],IF(Table1[[#This Row],[3]]&lt;&gt;"",Table1[[#This Row],[3]],"-")))</calculatedColumnFormula>
+      <totalsRowFormula>"[0"&amp;","&amp;E2&amp;","&amp;E3&amp;","&amp;E4&amp;","&amp;E5&amp;","&amp;E6&amp;","&amp;E7&amp;","&amp;E8&amp;","&amp;E9&amp;","&amp;E10&amp;","&amp;E11&amp;","&amp;E12&amp;","&amp;E13&amp;","&amp;E14&amp;","&amp;E15&amp;","&amp;E16&amp;","&amp;E17&amp;","&amp;E18&amp;","&amp;E19&amp;","&amp;E20&amp;","&amp;E21&amp;","&amp;E22&amp;","&amp;E23&amp;","&amp;E24&amp;","&amp;E25&amp;","&amp;E26&amp;"]"</totalsRowFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CAFE9AE5-0B16-4514-B197-572F13AA30A7}" name="Table134" displayName="Table134" ref="A1:E27" totalsRowCount="1" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:E26" xr:uid="{C9AE075E-B9D0-44B1-A335-E02B884B531E}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{EF4F8265-B0FC-41E6-8AC1-651C4897F2CA}" name="0"/>
+    <tableColumn id="2" xr3:uid="{F55FCA69-A470-4417-96D6-371FADAD369E}" name="1" dataDxfId="7" totalsRowDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{1F9511D4-2006-44BE-92C1-B633CA778DFD}" name="2" dataDxfId="6" totalsRowDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{1115CEC8-FF8F-4254-B621-91D36AC9C5CA}" name="3" dataDxfId="5" totalsRowDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{089919ED-3EAD-4973-82E9-8D6B7131EB45}" name="FULL" totalsRowFunction="custom" dataDxfId="4" totalsRowDxfId="0">
+      <calculatedColumnFormula>IF(Table134[[#This Row],[1]]&lt;&gt;"",Table134[[#This Row],[1]],IF(Table134[[#This Row],[2]]&lt;&gt;"",Table134[[#This Row],[2]],IF(Table134[[#This Row],[3]]&lt;&gt;"",Table134[[#This Row],[3]],"-")))</calculatedColumnFormula>
       <totalsRowFormula>"[0"&amp;","&amp;E2&amp;","&amp;E3&amp;","&amp;E4&amp;","&amp;E5&amp;","&amp;E6&amp;","&amp;E7&amp;","&amp;E8&amp;","&amp;E9&amp;","&amp;E10&amp;","&amp;E11&amp;","&amp;E12&amp;","&amp;E13&amp;","&amp;E14&amp;","&amp;E15&amp;","&amp;E16&amp;","&amp;E17&amp;","&amp;E18&amp;","&amp;E19&amp;","&amp;E20&amp;","&amp;E21&amp;","&amp;E22&amp;","&amp;E23&amp;","&amp;E24&amp;","&amp;E25&amp;","&amp;E26&amp;"]"</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -1359,7 +1568,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A26"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1808,6 +2017,467 @@
       <c r="E27" s="3" t="str">
         <f>"[0"&amp;","&amp;E2&amp;","&amp;E3&amp;","&amp;E4&amp;","&amp;E5&amp;","&amp;E6&amp;","&amp;E7&amp;","&amp;E8&amp;","&amp;E9&amp;","&amp;E10&amp;","&amp;E11&amp;","&amp;E12&amp;","&amp;E13&amp;","&amp;E14&amp;","&amp;E15&amp;","&amp;E16&amp;","&amp;E17&amp;","&amp;E18&amp;","&amp;E19&amp;","&amp;E20&amp;","&amp;E21&amp;","&amp;E22&amp;","&amp;E23&amp;","&amp;E24&amp;","&amp;E25&amp;","&amp;E26&amp;"]"</f>
         <v>[0,3,1,1,1,1,3,3,3,2,3,1,2,1,1,1,2,1,1,2,1,2,1,1,1,1]</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB2A6C6-C582-4C85-A787-E6B26E995BE3}">
+  <dimension ref="A1:E27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1">
+        <f>IF(Table134[[#This Row],[1]]&lt;&gt;"",Table134[[#This Row],[1]],IF(Table134[[#This Row],[2]]&lt;&gt;"",Table134[[#This Row],[2]],IF(Table134[[#This Row],[3]]&lt;&gt;"",Table134[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1">
+        <f>IF(Table134[[#This Row],[1]]&lt;&gt;"",Table134[[#This Row],[1]],IF(Table134[[#This Row],[2]]&lt;&gt;"",Table134[[#This Row],[2]],IF(Table134[[#This Row],[3]]&lt;&gt;"",Table134[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="5">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1">
+        <f>IF(Table134[[#This Row],[1]]&lt;&gt;"",Table134[[#This Row],[1]],IF(Table134[[#This Row],[2]]&lt;&gt;"",Table134[[#This Row],[2]],IF(Table134[[#This Row],[3]]&lt;&gt;"",Table134[[#This Row],[3]],"-")))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="6">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1">
+        <f>IF(Table134[[#This Row],[1]]&lt;&gt;"",Table134[[#This Row],[1]],IF(Table134[[#This Row],[2]]&lt;&gt;"",Table134[[#This Row],[2]],IF(Table134[[#This Row],[3]]&lt;&gt;"",Table134[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="5">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1">
+        <f>IF(Table134[[#This Row],[1]]&lt;&gt;"",Table134[[#This Row],[1]],IF(Table134[[#This Row],[2]]&lt;&gt;"",Table134[[#This Row],[2]],IF(Table134[[#This Row],[3]]&lt;&gt;"",Table134[[#This Row],[3]],"-")))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="5">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1">
+        <f>IF(Table134[[#This Row],[1]]&lt;&gt;"",Table134[[#This Row],[1]],IF(Table134[[#This Row],[2]]&lt;&gt;"",Table134[[#This Row],[2]],IF(Table134[[#This Row],[3]]&lt;&gt;"",Table134[[#This Row],[3]],"-")))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1</v>
+      </c>
+      <c r="C8" s="6">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1">
+        <f>IF(Table134[[#This Row],[1]]&lt;&gt;"",Table134[[#This Row],[1]],IF(Table134[[#This Row],[2]]&lt;&gt;"",Table134[[#This Row],[2]],IF(Table134[[#This Row],[3]]&lt;&gt;"",Table134[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="5">
+        <v>2</v>
+      </c>
+      <c r="D9" s="6">
+        <v>3</v>
+      </c>
+      <c r="E9" s="1">
+        <f>IF(Table134[[#This Row],[1]]&lt;&gt;"",Table134[[#This Row],[1]],IF(Table134[[#This Row],[2]]&lt;&gt;"",Table134[[#This Row],[2]],IF(Table134[[#This Row],[3]]&lt;&gt;"",Table134[[#This Row],[3]],"-")))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="5">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1">
+        <f>IF(Table134[[#This Row],[1]]&lt;&gt;"",Table134[[#This Row],[1]],IF(Table134[[#This Row],[2]]&lt;&gt;"",Table134[[#This Row],[2]],IF(Table134[[#This Row],[3]]&lt;&gt;"",Table134[[#This Row],[3]],"-")))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5">
+        <v>1</v>
+      </c>
+      <c r="C11" s="6">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>3</v>
+      </c>
+      <c r="E11" s="1">
+        <f>IF(Table134[[#This Row],[1]]&lt;&gt;"",Table134[[#This Row],[1]],IF(Table134[[#This Row],[2]]&lt;&gt;"",Table134[[#This Row],[2]],IF(Table134[[#This Row],[3]]&lt;&gt;"",Table134[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="5">
+        <v>3</v>
+      </c>
+      <c r="E12" s="1">
+        <f>IF(Table134[[#This Row],[1]]&lt;&gt;"",Table134[[#This Row],[1]],IF(Table134[[#This Row],[2]]&lt;&gt;"",Table134[[#This Row],[2]],IF(Table134[[#This Row],[3]]&lt;&gt;"",Table134[[#This Row],[3]],"-")))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5">
+        <v>1</v>
+      </c>
+      <c r="C13" s="6">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1">
+        <f>IF(Table134[[#This Row],[1]]&lt;&gt;"",Table134[[#This Row],[1]],IF(Table134[[#This Row],[2]]&lt;&gt;"",Table134[[#This Row],[2]],IF(Table134[[#This Row],[3]]&lt;&gt;"",Table134[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="5">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1">
+        <f>IF(Table134[[#This Row],[1]]&lt;&gt;"",Table134[[#This Row],[1]],IF(Table134[[#This Row],[2]]&lt;&gt;"",Table134[[#This Row],[2]],IF(Table134[[#This Row],[3]]&lt;&gt;"",Table134[[#This Row],[3]],"-")))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="5">
+        <v>3</v>
+      </c>
+      <c r="E15" s="1">
+        <f>IF(Table134[[#This Row],[1]]&lt;&gt;"",Table134[[#This Row],[1]],IF(Table134[[#This Row],[2]]&lt;&gt;"",Table134[[#This Row],[2]],IF(Table134[[#This Row],[3]]&lt;&gt;"",Table134[[#This Row],[3]],"-")))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="5">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1">
+        <v>3</v>
+      </c>
+      <c r="E16" s="1">
+        <f>IF(Table134[[#This Row],[1]]&lt;&gt;"",Table134[[#This Row],[1]],IF(Table134[[#This Row],[2]]&lt;&gt;"",Table134[[#This Row],[2]],IF(Table134[[#This Row],[3]]&lt;&gt;"",Table134[[#This Row],[3]],"-")))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="5">
+        <v>2</v>
+      </c>
+      <c r="D17" s="1">
+        <v>3</v>
+      </c>
+      <c r="E17" s="1">
+        <f>IF(Table134[[#This Row],[1]]&lt;&gt;"",Table134[[#This Row],[1]],IF(Table134[[#This Row],[2]]&lt;&gt;"",Table134[[#This Row],[2]],IF(Table134[[#This Row],[3]]&lt;&gt;"",Table134[[#This Row],[3]],"-")))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="5">
+        <v>3</v>
+      </c>
+      <c r="E18" s="1">
+        <f>IF(Table134[[#This Row],[1]]&lt;&gt;"",Table134[[#This Row],[1]],IF(Table134[[#This Row],[2]]&lt;&gt;"",Table134[[#This Row],[2]],IF(Table134[[#This Row],[3]]&lt;&gt;"",Table134[[#This Row],[3]],"-")))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="5">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>3</v>
+      </c>
+      <c r="E19" s="1">
+        <f>IF(Table134[[#This Row],[1]]&lt;&gt;"",Table134[[#This Row],[1]],IF(Table134[[#This Row],[2]]&lt;&gt;"",Table134[[#This Row],[2]],IF(Table134[[#This Row],[3]]&lt;&gt;"",Table134[[#This Row],[3]],"-")))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5">
+        <v>1</v>
+      </c>
+      <c r="C20" s="6">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1">
+        <v>3</v>
+      </c>
+      <c r="E20" s="1">
+        <f>IF(Table134[[#This Row],[1]]&lt;&gt;"",Table134[[#This Row],[1]],IF(Table134[[#This Row],[2]]&lt;&gt;"",Table134[[#This Row],[2]],IF(Table134[[#This Row],[3]]&lt;&gt;"",Table134[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5">
+        <v>1</v>
+      </c>
+      <c r="C21" s="6">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>3</v>
+      </c>
+      <c r="E21" s="1">
+        <f>IF(Table134[[#This Row],[1]]&lt;&gt;"",Table134[[#This Row],[1]],IF(Table134[[#This Row],[2]]&lt;&gt;"",Table134[[#This Row],[2]],IF(Table134[[#This Row],[3]]&lt;&gt;"",Table134[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="5">
+        <v>2</v>
+      </c>
+      <c r="D22" s="1">
+        <v>3</v>
+      </c>
+      <c r="E22" s="1">
+        <f>IF(Table134[[#This Row],[1]]&lt;&gt;"",Table134[[#This Row],[1]],IF(Table134[[#This Row],[2]]&lt;&gt;"",Table134[[#This Row],[2]],IF(Table134[[#This Row],[3]]&lt;&gt;"",Table134[[#This Row],[3]],"-")))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6">
+        <v>1</v>
+      </c>
+      <c r="C23" s="6">
+        <v>2</v>
+      </c>
+      <c r="D23" s="1">
+        <v>3</v>
+      </c>
+      <c r="E23" s="1">
+        <f>IF(Table134[[#This Row],[1]]&lt;&gt;"",Table134[[#This Row],[1]],IF(Table134[[#This Row],[2]]&lt;&gt;"",Table134[[#This Row],[2]],IF(Table134[[#This Row],[3]]&lt;&gt;"",Table134[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" s="1">
+        <v>3</v>
+      </c>
+      <c r="E24" s="1">
+        <f>IF(Table134[[#This Row],[1]]&lt;&gt;"",Table134[[#This Row],[1]],IF(Table134[[#This Row],[2]]&lt;&gt;"",Table134[[#This Row],[2]],IF(Table134[[#This Row],[3]]&lt;&gt;"",Table134[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2</v>
+      </c>
+      <c r="D25" s="1">
+        <v>3</v>
+      </c>
+      <c r="E25" s="1">
+        <f>IF(Table134[[#This Row],[1]]&lt;&gt;"",Table134[[#This Row],[1]],IF(Table134[[#This Row],[2]]&lt;&gt;"",Table134[[#This Row],[2]],IF(Table134[[#This Row],[3]]&lt;&gt;"",Table134[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1">
+        <v>2</v>
+      </c>
+      <c r="D26" s="1">
+        <v>3</v>
+      </c>
+      <c r="E26" s="1">
+        <f>IF(Table134[[#This Row],[1]]&lt;&gt;"",Table134[[#This Row],[1]],IF(Table134[[#This Row],[2]]&lt;&gt;"",Table134[[#This Row],[2]],IF(Table134[[#This Row],[3]]&lt;&gt;"",Table134[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="3" t="str">
+        <f>"[0"&amp;","&amp;E2&amp;","&amp;E3&amp;","&amp;E4&amp;","&amp;E5&amp;","&amp;E6&amp;","&amp;E7&amp;","&amp;E8&amp;","&amp;E9&amp;","&amp;E10&amp;","&amp;E11&amp;","&amp;E12&amp;","&amp;E13&amp;","&amp;E14&amp;","&amp;E15&amp;","&amp;E16&amp;","&amp;E17&amp;","&amp;E18&amp;","&amp;E19&amp;","&amp;E20&amp;","&amp;E21&amp;","&amp;E22&amp;","&amp;E23&amp;","&amp;E24&amp;","&amp;E25&amp;","&amp;E26&amp;"]"</f>
+        <v>[0,1,1,2,1,2,3,1,2,2,1,3,1,2,3,2,2,3,2,1,1,2,1,1,1,1]</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update for Speed Quiz 2023-05-12
</commit_message>
<xml_diff>
--- a/scripts/QuizConfigHelper.xlsx
+++ b/scripts/QuizConfigHelper.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrej\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5BC39A-1063-4EAA-A0B7-4F0461C426BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{371B0742-2774-4F6B-8B2F-A9906FE1F607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1995" windowWidth="29040" windowHeight="17640" xr2:uid="{1A1E301B-5405-4BF5-94E3-74BAFB9EEE14}"/>
+    <workbookView xWindow="-28920" yWindow="-1845" windowWidth="29040" windowHeight="17640" xr2:uid="{1A1E301B-5405-4BF5-94E3-74BAFB9EEE14}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="2" r:id="rId1"/>
     <sheet name="2023-5-5" sheetId="1" r:id="rId2"/>
     <sheet name="2023-5-9" sheetId="3" r:id="rId3"/>
+    <sheet name="2023-05-12" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="10">
   <si>
     <t>0</t>
   </si>
@@ -139,7 +140,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="40">
     <dxf>
       <font>
         <b val="0"/>
@@ -231,6 +232,188 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -700,14 +883,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{95E507F7-1E07-427A-A363-C0FB487EC785}" name="Table13" displayName="Table13" ref="A1:E27" totalsRowCount="1" headerRowDxfId="29" dataDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{95E507F7-1E07-427A-A363-C0FB487EC785}" name="Table13" displayName="Table13" ref="A1:E27" totalsRowCount="1" headerRowDxfId="39" dataDxfId="38">
   <autoFilter ref="A1:E26" xr:uid="{C9AE075E-B9D0-44B1-A335-E02B884B531E}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{C69BBE94-502E-47D3-A9AA-F194F354155A}" name="0"/>
-    <tableColumn id="2" xr3:uid="{1FB0E793-A471-497D-88C4-949E9BFA0C8F}" name="1" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{89F2C03D-ED22-4063-911D-E7373DEF9496}" name="2" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{1FA3B4D5-8641-4F49-9616-E0366217905E}" name="3" dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{91B96506-156E-4C32-99E8-0DE63DDC8C37}" name="FULL" totalsRowFunction="custom" dataDxfId="21" totalsRowDxfId="20">
+    <tableColumn id="2" xr3:uid="{1FB0E793-A471-497D-88C4-949E9BFA0C8F}" name="1" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{89F2C03D-ED22-4063-911D-E7373DEF9496}" name="2" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{1FA3B4D5-8641-4F49-9616-E0366217905E}" name="3" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{91B96506-156E-4C32-99E8-0DE63DDC8C37}" name="FULL" totalsRowFunction="custom" dataDxfId="31" totalsRowDxfId="30">
       <calculatedColumnFormula>IF(Table13[[#This Row],[1]]&lt;&gt;"",Table13[[#This Row],[1]],IF(Table13[[#This Row],[2]]&lt;&gt;"",Table13[[#This Row],[2]],IF(Table13[[#This Row],[3]]&lt;&gt;"",Table13[[#This Row],[3]],"-")))</calculatedColumnFormula>
       <totalsRowFormula>"[0"&amp;","&amp;E2&amp;","&amp;E3&amp;","&amp;E4&amp;","&amp;E5&amp;","&amp;E6&amp;","&amp;E7&amp;","&amp;E8&amp;","&amp;E9&amp;","&amp;E10&amp;","&amp;E11&amp;","&amp;E12&amp;","&amp;E13&amp;","&amp;E14&amp;","&amp;E15&amp;","&amp;E16&amp;","&amp;E17&amp;","&amp;E18&amp;","&amp;E19&amp;","&amp;E20&amp;","&amp;E21&amp;","&amp;E22&amp;","&amp;E23&amp;","&amp;E24&amp;","&amp;E25&amp;","&amp;E26&amp;"]"</totalsRowFormula>
     </tableColumn>
@@ -717,14 +900,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C9AE075E-B9D0-44B1-A335-E02B884B531E}" name="Table1" displayName="Table1" ref="A1:E27" totalsRowCount="1" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C9AE075E-B9D0-44B1-A335-E02B884B531E}" name="Table1" displayName="Table1" ref="A1:E27" totalsRowCount="1" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="A1:E26" xr:uid="{C9AE075E-B9D0-44B1-A335-E02B884B531E}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{DCFB1B30-AA68-4524-AF80-5AFE18AC05BB}" name="0"/>
-    <tableColumn id="2" xr3:uid="{A90B6EEB-FC8B-4231-A5E2-A31293EDB551}" name="1" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{585B8F47-B526-4C76-86B8-BE40EFC8C722}" name="2" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{54B78388-3C67-4184-9ECE-F5B91C34B9B0}" name="3" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{8EAC5146-454C-4D49-93CC-6E35149D5DE1}" name="FULL" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="10">
+    <tableColumn id="2" xr3:uid="{A90B6EEB-FC8B-4231-A5E2-A31293EDB551}" name="1" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{585B8F47-B526-4C76-86B8-BE40EFC8C722}" name="2" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{54B78388-3C67-4184-9ECE-F5B91C34B9B0}" name="3" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{8EAC5146-454C-4D49-93CC-6E35149D5DE1}" name="FULL" totalsRowFunction="custom" dataDxfId="21" totalsRowDxfId="20">
       <calculatedColumnFormula>IF(Table1[[#This Row],[1]]&lt;&gt;"",Table1[[#This Row],[1]],IF(Table1[[#This Row],[2]]&lt;&gt;"",Table1[[#This Row],[2]],IF(Table1[[#This Row],[3]]&lt;&gt;"",Table1[[#This Row],[3]],"-")))</calculatedColumnFormula>
       <totalsRowFormula>"[0"&amp;","&amp;E2&amp;","&amp;E3&amp;","&amp;E4&amp;","&amp;E5&amp;","&amp;E6&amp;","&amp;E7&amp;","&amp;E8&amp;","&amp;E9&amp;","&amp;E10&amp;","&amp;E11&amp;","&amp;E12&amp;","&amp;E13&amp;","&amp;E14&amp;","&amp;E15&amp;","&amp;E16&amp;","&amp;E17&amp;","&amp;E18&amp;","&amp;E19&amp;","&amp;E20&amp;","&amp;E21&amp;","&amp;E22&amp;","&amp;E23&amp;","&amp;E24&amp;","&amp;E25&amp;","&amp;E26&amp;"]"</totalsRowFormula>
     </tableColumn>
@@ -734,15 +917,32 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CAFE9AE5-0B16-4514-B197-572F13AA30A7}" name="Table134" displayName="Table134" ref="A1:E27" totalsRowCount="1" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CAFE9AE5-0B16-4514-B197-572F13AA30A7}" name="Table134" displayName="Table134" ref="A1:E27" totalsRowCount="1" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A1:E26" xr:uid="{C9AE075E-B9D0-44B1-A335-E02B884B531E}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{EF4F8265-B0FC-41E6-8AC1-651C4897F2CA}" name="0"/>
-    <tableColumn id="2" xr3:uid="{F55FCA69-A470-4417-96D6-371FADAD369E}" name="1" dataDxfId="7" totalsRowDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{1F9511D4-2006-44BE-92C1-B633CA778DFD}" name="2" dataDxfId="6" totalsRowDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{1115CEC8-FF8F-4254-B621-91D36AC9C5CA}" name="3" dataDxfId="5" totalsRowDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{089919ED-3EAD-4973-82E9-8D6B7131EB45}" name="FULL" totalsRowFunction="custom" dataDxfId="4" totalsRowDxfId="0">
+    <tableColumn id="2" xr3:uid="{F55FCA69-A470-4417-96D6-371FADAD369E}" name="1" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{1F9511D4-2006-44BE-92C1-B633CA778DFD}" name="2" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{1115CEC8-FF8F-4254-B621-91D36AC9C5CA}" name="3" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{089919ED-3EAD-4973-82E9-8D6B7131EB45}" name="FULL" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="10">
       <calculatedColumnFormula>IF(Table134[[#This Row],[1]]&lt;&gt;"",Table134[[#This Row],[1]],IF(Table134[[#This Row],[2]]&lt;&gt;"",Table134[[#This Row],[2]],IF(Table134[[#This Row],[3]]&lt;&gt;"",Table134[[#This Row],[3]],"-")))</calculatedColumnFormula>
+      <totalsRowFormula>"[0"&amp;","&amp;E2&amp;","&amp;E3&amp;","&amp;E4&amp;","&amp;E5&amp;","&amp;E6&amp;","&amp;E7&amp;","&amp;E8&amp;","&amp;E9&amp;","&amp;E10&amp;","&amp;E11&amp;","&amp;E12&amp;","&amp;E13&amp;","&amp;E14&amp;","&amp;E15&amp;","&amp;E16&amp;","&amp;E17&amp;","&amp;E18&amp;","&amp;E19&amp;","&amp;E20&amp;","&amp;E21&amp;","&amp;E22&amp;","&amp;E23&amp;","&amp;E24&amp;","&amp;E25&amp;","&amp;E26&amp;"]"</totalsRowFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CEC9C3D7-EE85-4DF0-AA68-D5AD46CF29E5}" name="Table135" displayName="Table135" ref="A1:E27" totalsRowCount="1" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:E26" xr:uid="{C9AE075E-B9D0-44B1-A335-E02B884B531E}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{505F929E-768B-4C6A-8319-02D7AF42B437}" name="0"/>
+    <tableColumn id="2" xr3:uid="{6EFB68BD-9CE4-4AF7-AF18-1466AB5D36AC}" name="1" dataDxfId="7" totalsRowDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{D2E9260F-FA42-4A89-BF27-AB9FDCF0C09D}" name="2" dataDxfId="6" totalsRowDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{3C83FC51-5AEB-45FA-BDF8-E7301DB8B532}" name="3" dataDxfId="5" totalsRowDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{732009B5-960E-4EA9-A36A-0FC6CC36741E}" name="FULL" totalsRowFunction="custom" dataDxfId="4" totalsRowDxfId="0">
+      <calculatedColumnFormula>IF(Table135[[#This Row],[1]]&lt;&gt;"",Table135[[#This Row],[1]],IF(Table135[[#This Row],[2]]&lt;&gt;"",Table135[[#This Row],[2]],IF(Table135[[#This Row],[3]]&lt;&gt;"",Table135[[#This Row],[3]],"-")))</calculatedColumnFormula>
       <totalsRowFormula>"[0"&amp;","&amp;E2&amp;","&amp;E3&amp;","&amp;E4&amp;","&amp;E5&amp;","&amp;E6&amp;","&amp;E7&amp;","&amp;E8&amp;","&amp;E9&amp;","&amp;E10&amp;","&amp;E11&amp;","&amp;E12&amp;","&amp;E13&amp;","&amp;E14&amp;","&amp;E15&amp;","&amp;E16&amp;","&amp;E17&amp;","&amp;E18&amp;","&amp;E19&amp;","&amp;E20&amp;","&amp;E21&amp;","&amp;E22&amp;","&amp;E23&amp;","&amp;E24&amp;","&amp;E25&amp;","&amp;E26&amp;"]"</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -2487,4 +2687,465 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26833DCF-168B-408E-878D-5DFA53F24BA0}">
+  <dimension ref="A1:E27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1">
+        <f>IF(Table135[[#This Row],[1]]&lt;&gt;"",Table135[[#This Row],[1]],IF(Table135[[#This Row],[2]]&lt;&gt;"",Table135[[#This Row],[2]],IF(Table135[[#This Row],[3]]&lt;&gt;"",Table135[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="5">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1">
+        <f>IF(Table135[[#This Row],[1]]&lt;&gt;"",Table135[[#This Row],[1]],IF(Table135[[#This Row],[2]]&lt;&gt;"",Table135[[#This Row],[2]],IF(Table135[[#This Row],[3]]&lt;&gt;"",Table135[[#This Row],[3]],"-")))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1">
+        <f>IF(Table135[[#This Row],[1]]&lt;&gt;"",Table135[[#This Row],[1]],IF(Table135[[#This Row],[2]]&lt;&gt;"",Table135[[#This Row],[2]],IF(Table135[[#This Row],[3]]&lt;&gt;"",Table135[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1">
+        <f>IF(Table135[[#This Row],[1]]&lt;&gt;"",Table135[[#This Row],[1]],IF(Table135[[#This Row],[2]]&lt;&gt;"",Table135[[#This Row],[2]],IF(Table135[[#This Row],[3]]&lt;&gt;"",Table135[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="5">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1">
+        <f>IF(Table135[[#This Row],[1]]&lt;&gt;"",Table135[[#This Row],[1]],IF(Table135[[#This Row],[2]]&lt;&gt;"",Table135[[#This Row],[2]],IF(Table135[[#This Row],[3]]&lt;&gt;"",Table135[[#This Row],[3]],"-")))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="5">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1">
+        <f>IF(Table135[[#This Row],[1]]&lt;&gt;"",Table135[[#This Row],[1]],IF(Table135[[#This Row],[2]]&lt;&gt;"",Table135[[#This Row],[2]],IF(Table135[[#This Row],[3]]&lt;&gt;"",Table135[[#This Row],[3]],"-")))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="5">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1">
+        <f>IF(Table135[[#This Row],[1]]&lt;&gt;"",Table135[[#This Row],[1]],IF(Table135[[#This Row],[2]]&lt;&gt;"",Table135[[#This Row],[2]],IF(Table135[[#This Row],[3]]&lt;&gt;"",Table135[[#This Row],[3]],"-")))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="5">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>3</v>
+      </c>
+      <c r="E9" s="1">
+        <f>IF(Table135[[#This Row],[1]]&lt;&gt;"",Table135[[#This Row],[1]],IF(Table135[[#This Row],[2]]&lt;&gt;"",Table135[[#This Row],[2]],IF(Table135[[#This Row],[3]]&lt;&gt;"",Table135[[#This Row],[3]],"-")))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="5">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1">
+        <f>IF(Table135[[#This Row],[1]]&lt;&gt;"",Table135[[#This Row],[1]],IF(Table135[[#This Row],[2]]&lt;&gt;"",Table135[[#This Row],[2]],IF(Table135[[#This Row],[3]]&lt;&gt;"",Table135[[#This Row],[3]],"-")))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>3</v>
+      </c>
+      <c r="E11" s="1">
+        <f>IF(Table135[[#This Row],[1]]&lt;&gt;"",Table135[[#This Row],[1]],IF(Table135[[#This Row],[2]]&lt;&gt;"",Table135[[#This Row],[2]],IF(Table135[[#This Row],[3]]&lt;&gt;"",Table135[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1">
+        <v>3</v>
+      </c>
+      <c r="E12" s="1">
+        <f>IF(Table135[[#This Row],[1]]&lt;&gt;"",Table135[[#This Row],[1]],IF(Table135[[#This Row],[2]]&lt;&gt;"",Table135[[#This Row],[2]],IF(Table135[[#This Row],[3]]&lt;&gt;"",Table135[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1">
+        <f>IF(Table135[[#This Row],[1]]&lt;&gt;"",Table135[[#This Row],[1]],IF(Table135[[#This Row],[2]]&lt;&gt;"",Table135[[#This Row],[2]],IF(Table135[[#This Row],[3]]&lt;&gt;"",Table135[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="5">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1">
+        <f>IF(Table135[[#This Row],[1]]&lt;&gt;"",Table135[[#This Row],[1]],IF(Table135[[#This Row],[2]]&lt;&gt;"",Table135[[#This Row],[2]],IF(Table135[[#This Row],[3]]&lt;&gt;"",Table135[[#This Row],[3]],"-")))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>3</v>
+      </c>
+      <c r="E15" s="1">
+        <f>IF(Table135[[#This Row],[1]]&lt;&gt;"",Table135[[#This Row],[1]],IF(Table135[[#This Row],[2]]&lt;&gt;"",Table135[[#This Row],[2]],IF(Table135[[#This Row],[3]]&lt;&gt;"",Table135[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="5">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1">
+        <v>3</v>
+      </c>
+      <c r="E16" s="1">
+        <f>IF(Table135[[#This Row],[1]]&lt;&gt;"",Table135[[#This Row],[1]],IF(Table135[[#This Row],[2]]&lt;&gt;"",Table135[[#This Row],[2]],IF(Table135[[#This Row],[3]]&lt;&gt;"",Table135[[#This Row],[3]],"-")))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="5">
+        <v>3</v>
+      </c>
+      <c r="E17" s="1">
+        <f>IF(Table135[[#This Row],[1]]&lt;&gt;"",Table135[[#This Row],[1]],IF(Table135[[#This Row],[2]]&lt;&gt;"",Table135[[#This Row],[2]],IF(Table135[[#This Row],[3]]&lt;&gt;"",Table135[[#This Row],[3]],"-")))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2</v>
+      </c>
+      <c r="D18" s="1">
+        <v>3</v>
+      </c>
+      <c r="E18" s="1">
+        <f>IF(Table135[[#This Row],[1]]&lt;&gt;"",Table135[[#This Row],[1]],IF(Table135[[#This Row],[2]]&lt;&gt;"",Table135[[#This Row],[2]],IF(Table135[[#This Row],[3]]&lt;&gt;"",Table135[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="5">
+        <v>3</v>
+      </c>
+      <c r="E19" s="1">
+        <f>IF(Table135[[#This Row],[1]]&lt;&gt;"",Table135[[#This Row],[1]],IF(Table135[[#This Row],[2]]&lt;&gt;"",Table135[[#This Row],[2]],IF(Table135[[#This Row],[3]]&lt;&gt;"",Table135[[#This Row],[3]],"-")))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1">
+        <v>3</v>
+      </c>
+      <c r="E20" s="1">
+        <f>IF(Table135[[#This Row],[1]]&lt;&gt;"",Table135[[#This Row],[1]],IF(Table135[[#This Row],[2]]&lt;&gt;"",Table135[[#This Row],[2]],IF(Table135[[#This Row],[3]]&lt;&gt;"",Table135[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>3</v>
+      </c>
+      <c r="E21" s="1">
+        <f>IF(Table135[[#This Row],[1]]&lt;&gt;"",Table135[[#This Row],[1]],IF(Table135[[#This Row],[2]]&lt;&gt;"",Table135[[#This Row],[2]],IF(Table135[[#This Row],[3]]&lt;&gt;"",Table135[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="5">
+        <v>2</v>
+      </c>
+      <c r="D22" s="1">
+        <v>3</v>
+      </c>
+      <c r="E22" s="1">
+        <f>IF(Table135[[#This Row],[1]]&lt;&gt;"",Table135[[#This Row],[1]],IF(Table135[[#This Row],[2]]&lt;&gt;"",Table135[[#This Row],[2]],IF(Table135[[#This Row],[3]]&lt;&gt;"",Table135[[#This Row],[3]],"-")))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1">
+        <v>2</v>
+      </c>
+      <c r="D23" s="1">
+        <v>3</v>
+      </c>
+      <c r="E23" s="1">
+        <f>IF(Table135[[#This Row],[1]]&lt;&gt;"",Table135[[#This Row],[1]],IF(Table135[[#This Row],[2]]&lt;&gt;"",Table135[[#This Row],[2]],IF(Table135[[#This Row],[3]]&lt;&gt;"",Table135[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" s="1">
+        <v>3</v>
+      </c>
+      <c r="E24" s="1">
+        <f>IF(Table135[[#This Row],[1]]&lt;&gt;"",Table135[[#This Row],[1]],IF(Table135[[#This Row],[2]]&lt;&gt;"",Table135[[#This Row],[2]],IF(Table135[[#This Row],[3]]&lt;&gt;"",Table135[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2</v>
+      </c>
+      <c r="D25" s="1">
+        <v>3</v>
+      </c>
+      <c r="E25" s="1">
+        <f>IF(Table135[[#This Row],[1]]&lt;&gt;"",Table135[[#This Row],[1]],IF(Table135[[#This Row],[2]]&lt;&gt;"",Table135[[#This Row],[2]],IF(Table135[[#This Row],[3]]&lt;&gt;"",Table135[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1">
+        <v>2</v>
+      </c>
+      <c r="D26" s="1">
+        <v>3</v>
+      </c>
+      <c r="E26" s="1">
+        <f>IF(Table135[[#This Row],[1]]&lt;&gt;"",Table135[[#This Row],[1]],IF(Table135[[#This Row],[2]]&lt;&gt;"",Table135[[#This Row],[2]],IF(Table135[[#This Row],[3]]&lt;&gt;"",Table135[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="3" t="str">
+        <f>"[0"&amp;","&amp;E2&amp;","&amp;E3&amp;","&amp;E4&amp;","&amp;E5&amp;","&amp;E6&amp;","&amp;E7&amp;","&amp;E8&amp;","&amp;E9&amp;","&amp;E10&amp;","&amp;E11&amp;","&amp;E12&amp;","&amp;E13&amp;","&amp;E14&amp;","&amp;E15&amp;","&amp;E16&amp;","&amp;E17&amp;","&amp;E18&amp;","&amp;E19&amp;","&amp;E20&amp;","&amp;E21&amp;","&amp;E22&amp;","&amp;E23&amp;","&amp;E24&amp;","&amp;E25&amp;","&amp;E26&amp;"]"</f>
+        <v>[0,1,3,1,1,2,3,3,2,2,1,1,1,2,1,2,3,1,3,1,1,2,1,1,1,1]</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update for Speed Quiz 2023-05-16
</commit_message>
<xml_diff>
--- a/scripts/QuizConfigHelper.xlsx
+++ b/scripts/QuizConfigHelper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrej\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{371B0742-2774-4F6B-8B2F-A9906FE1F607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{498647C1-9975-435A-A4EB-25D9F3EB4E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1845" windowWidth="29040" windowHeight="17640" xr2:uid="{1A1E301B-5405-4BF5-94E3-74BAFB9EEE14}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="2023-5-5" sheetId="1" r:id="rId2"/>
     <sheet name="2023-5-9" sheetId="3" r:id="rId3"/>
     <sheet name="2023-05-12" sheetId="4" r:id="rId4"/>
+    <sheet name="2023-05-16" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="15">
   <si>
     <t>0</t>
   </si>
@@ -68,12 +69,27 @@
   <si>
     <t>4. Do previous steps for all questions with ID 1-21</t>
   </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>1. Answer the question</t>
+  </si>
+  <si>
+    <t>2. In developer tools, Network - check for "challenges"</t>
+  </si>
+  <si>
+    <t>3. One request is for question number, another request (it's body) is for answer number</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,6 +106,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -127,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -136,11 +159,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="50">
     <dxf>
       <font>
         <b val="0"/>
@@ -232,6 +256,188 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -883,14 +1089,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{95E507F7-1E07-427A-A363-C0FB487EC785}" name="Table13" displayName="Table13" ref="A1:E27" totalsRowCount="1" headerRowDxfId="39" dataDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{95E507F7-1E07-427A-A363-C0FB487EC785}" name="Table13" displayName="Table13" ref="A1:E27" totalsRowCount="1" headerRowDxfId="49" dataDxfId="48">
   <autoFilter ref="A1:E26" xr:uid="{C9AE075E-B9D0-44B1-A335-E02B884B531E}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{C69BBE94-502E-47D3-A9AA-F194F354155A}" name="0"/>
-    <tableColumn id="2" xr3:uid="{1FB0E793-A471-497D-88C4-949E9BFA0C8F}" name="1" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{89F2C03D-ED22-4063-911D-E7373DEF9496}" name="2" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{1FA3B4D5-8641-4F49-9616-E0366217905E}" name="3" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{91B96506-156E-4C32-99E8-0DE63DDC8C37}" name="FULL" totalsRowFunction="custom" dataDxfId="31" totalsRowDxfId="30">
+    <tableColumn id="2" xr3:uid="{1FB0E793-A471-497D-88C4-949E9BFA0C8F}" name="1" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="3" xr3:uid="{89F2C03D-ED22-4063-911D-E7373DEF9496}" name="2" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{1FA3B4D5-8641-4F49-9616-E0366217905E}" name="3" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="5" xr3:uid="{91B96506-156E-4C32-99E8-0DE63DDC8C37}" name="FULL" totalsRowFunction="custom" dataDxfId="41" totalsRowDxfId="40">
       <calculatedColumnFormula>IF(Table13[[#This Row],[1]]&lt;&gt;"",Table13[[#This Row],[1]],IF(Table13[[#This Row],[2]]&lt;&gt;"",Table13[[#This Row],[2]],IF(Table13[[#This Row],[3]]&lt;&gt;"",Table13[[#This Row],[3]],"-")))</calculatedColumnFormula>
       <totalsRowFormula>"[0"&amp;","&amp;E2&amp;","&amp;E3&amp;","&amp;E4&amp;","&amp;E5&amp;","&amp;E6&amp;","&amp;E7&amp;","&amp;E8&amp;","&amp;E9&amp;","&amp;E10&amp;","&amp;E11&amp;","&amp;E12&amp;","&amp;E13&amp;","&amp;E14&amp;","&amp;E15&amp;","&amp;E16&amp;","&amp;E17&amp;","&amp;E18&amp;","&amp;E19&amp;","&amp;E20&amp;","&amp;E21&amp;","&amp;E22&amp;","&amp;E23&amp;","&amp;E24&amp;","&amp;E25&amp;","&amp;E26&amp;"]"</totalsRowFormula>
     </tableColumn>
@@ -900,14 +1106,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C9AE075E-B9D0-44B1-A335-E02B884B531E}" name="Table1" displayName="Table1" ref="A1:E27" totalsRowCount="1" headerRowDxfId="29" dataDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C9AE075E-B9D0-44B1-A335-E02B884B531E}" name="Table1" displayName="Table1" ref="A1:E27" totalsRowCount="1" headerRowDxfId="39" dataDxfId="38">
   <autoFilter ref="A1:E26" xr:uid="{C9AE075E-B9D0-44B1-A335-E02B884B531E}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{DCFB1B30-AA68-4524-AF80-5AFE18AC05BB}" name="0"/>
-    <tableColumn id="2" xr3:uid="{A90B6EEB-FC8B-4231-A5E2-A31293EDB551}" name="1" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{585B8F47-B526-4C76-86B8-BE40EFC8C722}" name="2" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{54B78388-3C67-4184-9ECE-F5B91C34B9B0}" name="3" dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{8EAC5146-454C-4D49-93CC-6E35149D5DE1}" name="FULL" totalsRowFunction="custom" dataDxfId="21" totalsRowDxfId="20">
+    <tableColumn id="2" xr3:uid="{A90B6EEB-FC8B-4231-A5E2-A31293EDB551}" name="1" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{585B8F47-B526-4C76-86B8-BE40EFC8C722}" name="2" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{54B78388-3C67-4184-9ECE-F5B91C34B9B0}" name="3" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{8EAC5146-454C-4D49-93CC-6E35149D5DE1}" name="FULL" totalsRowFunction="custom" dataDxfId="31" totalsRowDxfId="30">
       <calculatedColumnFormula>IF(Table1[[#This Row],[1]]&lt;&gt;"",Table1[[#This Row],[1]],IF(Table1[[#This Row],[2]]&lt;&gt;"",Table1[[#This Row],[2]],IF(Table1[[#This Row],[3]]&lt;&gt;"",Table1[[#This Row],[3]],"-")))</calculatedColumnFormula>
       <totalsRowFormula>"[0"&amp;","&amp;E2&amp;","&amp;E3&amp;","&amp;E4&amp;","&amp;E5&amp;","&amp;E6&amp;","&amp;E7&amp;","&amp;E8&amp;","&amp;E9&amp;","&amp;E10&amp;","&amp;E11&amp;","&amp;E12&amp;","&amp;E13&amp;","&amp;E14&amp;","&amp;E15&amp;","&amp;E16&amp;","&amp;E17&amp;","&amp;E18&amp;","&amp;E19&amp;","&amp;E20&amp;","&amp;E21&amp;","&amp;E22&amp;","&amp;E23&amp;","&amp;E24&amp;","&amp;E25&amp;","&amp;E26&amp;"]"</totalsRowFormula>
     </tableColumn>
@@ -917,14 +1123,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CAFE9AE5-0B16-4514-B197-572F13AA30A7}" name="Table134" displayName="Table134" ref="A1:E27" totalsRowCount="1" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CAFE9AE5-0B16-4514-B197-572F13AA30A7}" name="Table134" displayName="Table134" ref="A1:E27" totalsRowCount="1" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="A1:E26" xr:uid="{C9AE075E-B9D0-44B1-A335-E02B884B531E}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{EF4F8265-B0FC-41E6-8AC1-651C4897F2CA}" name="0"/>
-    <tableColumn id="2" xr3:uid="{F55FCA69-A470-4417-96D6-371FADAD369E}" name="1" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{1F9511D4-2006-44BE-92C1-B633CA778DFD}" name="2" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{1115CEC8-FF8F-4254-B621-91D36AC9C5CA}" name="3" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{089919ED-3EAD-4973-82E9-8D6B7131EB45}" name="FULL" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="10">
+    <tableColumn id="2" xr3:uid="{F55FCA69-A470-4417-96D6-371FADAD369E}" name="1" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{1F9511D4-2006-44BE-92C1-B633CA778DFD}" name="2" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{1115CEC8-FF8F-4254-B621-91D36AC9C5CA}" name="3" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{089919ED-3EAD-4973-82E9-8D6B7131EB45}" name="FULL" totalsRowFunction="custom" dataDxfId="21" totalsRowDxfId="20">
       <calculatedColumnFormula>IF(Table134[[#This Row],[1]]&lt;&gt;"",Table134[[#This Row],[1]],IF(Table134[[#This Row],[2]]&lt;&gt;"",Table134[[#This Row],[2]],IF(Table134[[#This Row],[3]]&lt;&gt;"",Table134[[#This Row],[3]],"-")))</calculatedColumnFormula>
       <totalsRowFormula>"[0"&amp;","&amp;E2&amp;","&amp;E3&amp;","&amp;E4&amp;","&amp;E5&amp;","&amp;E6&amp;","&amp;E7&amp;","&amp;E8&amp;","&amp;E9&amp;","&amp;E10&amp;","&amp;E11&amp;","&amp;E12&amp;","&amp;E13&amp;","&amp;E14&amp;","&amp;E15&amp;","&amp;E16&amp;","&amp;E17&amp;","&amp;E18&amp;","&amp;E19&amp;","&amp;E20&amp;","&amp;E21&amp;","&amp;E22&amp;","&amp;E23&amp;","&amp;E24&amp;","&amp;E25&amp;","&amp;E26&amp;"]"</totalsRowFormula>
     </tableColumn>
@@ -934,15 +1140,32 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CEC9C3D7-EE85-4DF0-AA68-D5AD46CF29E5}" name="Table135" displayName="Table135" ref="A1:E27" totalsRowCount="1" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CEC9C3D7-EE85-4DF0-AA68-D5AD46CF29E5}" name="Table135" displayName="Table135" ref="A1:E27" totalsRowCount="1" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A1:E26" xr:uid="{C9AE075E-B9D0-44B1-A335-E02B884B531E}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{505F929E-768B-4C6A-8319-02D7AF42B437}" name="0"/>
-    <tableColumn id="2" xr3:uid="{6EFB68BD-9CE4-4AF7-AF18-1466AB5D36AC}" name="1" dataDxfId="7" totalsRowDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{D2E9260F-FA42-4A89-BF27-AB9FDCF0C09D}" name="2" dataDxfId="6" totalsRowDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{3C83FC51-5AEB-45FA-BDF8-E7301DB8B532}" name="3" dataDxfId="5" totalsRowDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{732009B5-960E-4EA9-A36A-0FC6CC36741E}" name="FULL" totalsRowFunction="custom" dataDxfId="4" totalsRowDxfId="0">
+    <tableColumn id="2" xr3:uid="{6EFB68BD-9CE4-4AF7-AF18-1466AB5D36AC}" name="1" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{D2E9260F-FA42-4A89-BF27-AB9FDCF0C09D}" name="2" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{3C83FC51-5AEB-45FA-BDF8-E7301DB8B532}" name="3" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{732009B5-960E-4EA9-A36A-0FC6CC36741E}" name="FULL" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="10">
       <calculatedColumnFormula>IF(Table135[[#This Row],[1]]&lt;&gt;"",Table135[[#This Row],[1]],IF(Table135[[#This Row],[2]]&lt;&gt;"",Table135[[#This Row],[2]],IF(Table135[[#This Row],[3]]&lt;&gt;"",Table135[[#This Row],[3]],"-")))</calculatedColumnFormula>
+      <totalsRowFormula>"[0"&amp;","&amp;E2&amp;","&amp;E3&amp;","&amp;E4&amp;","&amp;E5&amp;","&amp;E6&amp;","&amp;E7&amp;","&amp;E8&amp;","&amp;E9&amp;","&amp;E10&amp;","&amp;E11&amp;","&amp;E12&amp;","&amp;E13&amp;","&amp;E14&amp;","&amp;E15&amp;","&amp;E16&amp;","&amp;E17&amp;","&amp;E18&amp;","&amp;E19&amp;","&amp;E20&amp;","&amp;E21&amp;","&amp;E22&amp;","&amp;E23&amp;","&amp;E24&amp;","&amp;E25&amp;","&amp;E26&amp;"]"</totalsRowFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0E0A6A52-5718-49B8-8795-73A4BFD1F483}" name="Table136" displayName="Table136" ref="A1:E27" totalsRowCount="1" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:E26" xr:uid="{C9AE075E-B9D0-44B1-A335-E02B884B531E}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{0C988102-ACAC-424A-87E2-5782013F7C30}" name="0"/>
+    <tableColumn id="2" xr3:uid="{4E69332C-5341-4C53-A801-A64D958F2603}" name="1" dataDxfId="7" totalsRowDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{867EDD1B-54AE-4A8C-A853-8A1EA8551A8D}" name="2" dataDxfId="6" totalsRowDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{3ECAF8E1-2961-4824-B5F3-E11CDDC98E0C}" name="3" dataDxfId="5" totalsRowDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{14CA4558-55D5-461C-A1B6-32348C9235E9}" name="FULL" totalsRowFunction="custom" dataDxfId="4" totalsRowDxfId="0">
+      <calculatedColumnFormula>IF(Table136[[#This Row],[1]]&lt;&gt;"",Table136[[#This Row],[1]],IF(Table136[[#This Row],[2]]&lt;&gt;"",Table136[[#This Row],[2]],IF(Table136[[#This Row],[3]]&lt;&gt;"",Table136[[#This Row],[3]],"-")))</calculatedColumnFormula>
       <totalsRowFormula>"[0"&amp;","&amp;E2&amp;","&amp;E3&amp;","&amp;E4&amp;","&amp;E5&amp;","&amp;E6&amp;","&amp;E7&amp;","&amp;E8&amp;","&amp;E9&amp;","&amp;E10&amp;","&amp;E11&amp;","&amp;E12&amp;","&amp;E13&amp;","&amp;E14&amp;","&amp;E15&amp;","&amp;E16&amp;","&amp;E17&amp;","&amp;E18&amp;","&amp;E19&amp;","&amp;E20&amp;","&amp;E21&amp;","&amp;E22&amp;","&amp;E23&amp;","&amp;E24&amp;","&amp;E25&amp;","&amp;E26&amp;"]"</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -1247,9 +1470,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2F98ED-1844-4978-B485-952E3D495531}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1729,6 +1954,11 @@
         <v>[0,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1,1]</v>
       </c>
     </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>5</v>
@@ -1752,6 +1982,26 @@
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -3148,4 +3398,465 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{387FBFF6-AFF5-4BA0-B8E8-3C6847664D38}">
+  <dimension ref="A1:E27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1">
+        <f>IF(Table136[[#This Row],[1]]&lt;&gt;"",Table136[[#This Row],[1]],IF(Table136[[#This Row],[2]]&lt;&gt;"",Table136[[#This Row],[2]],IF(Table136[[#This Row],[3]]&lt;&gt;"",Table136[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1">
+        <f>IF(Table136[[#This Row],[1]]&lt;&gt;"",Table136[[#This Row],[1]],IF(Table136[[#This Row],[2]]&lt;&gt;"",Table136[[#This Row],[2]],IF(Table136[[#This Row],[3]]&lt;&gt;"",Table136[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="8">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1">
+        <f>IF(Table136[[#This Row],[1]]&lt;&gt;"",Table136[[#This Row],[1]],IF(Table136[[#This Row],[2]]&lt;&gt;"",Table136[[#This Row],[2]],IF(Table136[[#This Row],[3]]&lt;&gt;"",Table136[[#This Row],[3]],"-")))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1">
+        <f>IF(Table136[[#This Row],[1]]&lt;&gt;"",Table136[[#This Row],[1]],IF(Table136[[#This Row],[2]]&lt;&gt;"",Table136[[#This Row],[2]],IF(Table136[[#This Row],[3]]&lt;&gt;"",Table136[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="8">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1">
+        <f>IF(Table136[[#This Row],[1]]&lt;&gt;"",Table136[[#This Row],[1]],IF(Table136[[#This Row],[2]]&lt;&gt;"",Table136[[#This Row],[2]],IF(Table136[[#This Row],[3]]&lt;&gt;"",Table136[[#This Row],[3]],"-")))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1">
+        <f>IF(Table136[[#This Row],[1]]&lt;&gt;"",Table136[[#This Row],[1]],IF(Table136[[#This Row],[2]]&lt;&gt;"",Table136[[#This Row],[2]],IF(Table136[[#This Row],[3]]&lt;&gt;"",Table136[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1">
+        <f>IF(Table136[[#This Row],[1]]&lt;&gt;"",Table136[[#This Row],[1]],IF(Table136[[#This Row],[2]]&lt;&gt;"",Table136[[#This Row],[2]],IF(Table136[[#This Row],[3]]&lt;&gt;"",Table136[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="8">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>3</v>
+      </c>
+      <c r="E9" s="1">
+        <f>IF(Table136[[#This Row],[1]]&lt;&gt;"",Table136[[#This Row],[1]],IF(Table136[[#This Row],[2]]&lt;&gt;"",Table136[[#This Row],[2]],IF(Table136[[#This Row],[3]]&lt;&gt;"",Table136[[#This Row],[3]],"-")))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="8">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1">
+        <f>IF(Table136[[#This Row],[1]]&lt;&gt;"",Table136[[#This Row],[1]],IF(Table136[[#This Row],[2]]&lt;&gt;"",Table136[[#This Row],[2]],IF(Table136[[#This Row],[3]]&lt;&gt;"",Table136[[#This Row],[3]],"-")))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>3</v>
+      </c>
+      <c r="E11" s="1">
+        <f>IF(Table136[[#This Row],[1]]&lt;&gt;"",Table136[[#This Row],[1]],IF(Table136[[#This Row],[2]]&lt;&gt;"",Table136[[#This Row],[2]],IF(Table136[[#This Row],[3]]&lt;&gt;"",Table136[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="8">
+        <v>3</v>
+      </c>
+      <c r="E12" s="1">
+        <f>IF(Table136[[#This Row],[1]]&lt;&gt;"",Table136[[#This Row],[1]],IF(Table136[[#This Row],[2]]&lt;&gt;"",Table136[[#This Row],[2]],IF(Table136[[#This Row],[3]]&lt;&gt;"",Table136[[#This Row],[3]],"-")))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="8">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1">
+        <f>IF(Table136[[#This Row],[1]]&lt;&gt;"",Table136[[#This Row],[1]],IF(Table136[[#This Row],[2]]&lt;&gt;"",Table136[[#This Row],[2]],IF(Table136[[#This Row],[3]]&lt;&gt;"",Table136[[#This Row],[3]],"-")))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="8">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1">
+        <f>IF(Table136[[#This Row],[1]]&lt;&gt;"",Table136[[#This Row],[1]],IF(Table136[[#This Row],[2]]&lt;&gt;"",Table136[[#This Row],[2]],IF(Table136[[#This Row],[3]]&lt;&gt;"",Table136[[#This Row],[3]],"-")))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="8">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1">
+        <v>3</v>
+      </c>
+      <c r="E15" s="1">
+        <f>IF(Table136[[#This Row],[1]]&lt;&gt;"",Table136[[#This Row],[1]],IF(Table136[[#This Row],[2]]&lt;&gt;"",Table136[[#This Row],[2]],IF(Table136[[#This Row],[3]]&lt;&gt;"",Table136[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="8">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1">
+        <v>3</v>
+      </c>
+      <c r="E16" s="1">
+        <f>IF(Table136[[#This Row],[1]]&lt;&gt;"",Table136[[#This Row],[1]],IF(Table136[[#This Row],[2]]&lt;&gt;"",Table136[[#This Row],[2]],IF(Table136[[#This Row],[3]]&lt;&gt;"",Table136[[#This Row],[3]],"-")))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="8">
+        <v>3</v>
+      </c>
+      <c r="E17" s="1">
+        <f>IF(Table136[[#This Row],[1]]&lt;&gt;"",Table136[[#This Row],[1]],IF(Table136[[#This Row],[2]]&lt;&gt;"",Table136[[#This Row],[2]],IF(Table136[[#This Row],[3]]&lt;&gt;"",Table136[[#This Row],[3]],"-")))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="8">
+        <v>3</v>
+      </c>
+      <c r="E18" s="1">
+        <f>IF(Table136[[#This Row],[1]]&lt;&gt;"",Table136[[#This Row],[1]],IF(Table136[[#This Row],[2]]&lt;&gt;"",Table136[[#This Row],[2]],IF(Table136[[#This Row],[3]]&lt;&gt;"",Table136[[#This Row],[3]],"-")))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="8">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>3</v>
+      </c>
+      <c r="E19" s="1">
+        <f>IF(Table136[[#This Row],[1]]&lt;&gt;"",Table136[[#This Row],[1]],IF(Table136[[#This Row],[2]]&lt;&gt;"",Table136[[#This Row],[2]],IF(Table136[[#This Row],[3]]&lt;&gt;"",Table136[[#This Row],[3]],"-")))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="8">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1">
+        <v>3</v>
+      </c>
+      <c r="E20" s="1">
+        <f>IF(Table136[[#This Row],[1]]&lt;&gt;"",Table136[[#This Row],[1]],IF(Table136[[#This Row],[2]]&lt;&gt;"",Table136[[#This Row],[2]],IF(Table136[[#This Row],[3]]&lt;&gt;"",Table136[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="8">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>3</v>
+      </c>
+      <c r="E21" s="1">
+        <f>IF(Table136[[#This Row],[1]]&lt;&gt;"",Table136[[#This Row],[1]],IF(Table136[[#This Row],[2]]&lt;&gt;"",Table136[[#This Row],[2]],IF(Table136[[#This Row],[3]]&lt;&gt;"",Table136[[#This Row],[3]],"-")))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="8">
+        <v>2</v>
+      </c>
+      <c r="D22" s="1">
+        <v>3</v>
+      </c>
+      <c r="E22" s="1">
+        <f>IF(Table136[[#This Row],[1]]&lt;&gt;"",Table136[[#This Row],[1]],IF(Table136[[#This Row],[2]]&lt;&gt;"",Table136[[#This Row],[2]],IF(Table136[[#This Row],[3]]&lt;&gt;"",Table136[[#This Row],[3]],"-")))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1">
+        <v>2</v>
+      </c>
+      <c r="D23" s="1">
+        <v>3</v>
+      </c>
+      <c r="E23" s="1">
+        <f>IF(Table136[[#This Row],[1]]&lt;&gt;"",Table136[[#This Row],[1]],IF(Table136[[#This Row],[2]]&lt;&gt;"",Table136[[#This Row],[2]],IF(Table136[[#This Row],[3]]&lt;&gt;"",Table136[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2</v>
+      </c>
+      <c r="D24" s="1">
+        <v>3</v>
+      </c>
+      <c r="E24" s="1">
+        <f>IF(Table136[[#This Row],[1]]&lt;&gt;"",Table136[[#This Row],[1]],IF(Table136[[#This Row],[2]]&lt;&gt;"",Table136[[#This Row],[2]],IF(Table136[[#This Row],[3]]&lt;&gt;"",Table136[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2</v>
+      </c>
+      <c r="D25" s="1">
+        <v>3</v>
+      </c>
+      <c r="E25" s="1">
+        <f>IF(Table136[[#This Row],[1]]&lt;&gt;"",Table136[[#This Row],[1]],IF(Table136[[#This Row],[2]]&lt;&gt;"",Table136[[#This Row],[2]],IF(Table136[[#This Row],[3]]&lt;&gt;"",Table136[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1">
+        <v>2</v>
+      </c>
+      <c r="D26" s="1">
+        <v>3</v>
+      </c>
+      <c r="E26" s="1">
+        <f>IF(Table136[[#This Row],[1]]&lt;&gt;"",Table136[[#This Row],[1]],IF(Table136[[#This Row],[2]]&lt;&gt;"",Table136[[#This Row],[2]],IF(Table136[[#This Row],[3]]&lt;&gt;"",Table136[[#This Row],[3]],"-")))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="3" t="str">
+        <f>"[0"&amp;","&amp;E2&amp;","&amp;E3&amp;","&amp;E4&amp;","&amp;E5&amp;","&amp;E6&amp;","&amp;E7&amp;","&amp;E8&amp;","&amp;E9&amp;","&amp;E10&amp;","&amp;E11&amp;","&amp;E12&amp;","&amp;E13&amp;","&amp;E14&amp;","&amp;E15&amp;","&amp;E16&amp;","&amp;E17&amp;","&amp;E18&amp;","&amp;E19&amp;","&amp;E20&amp;","&amp;E21&amp;","&amp;E22&amp;","&amp;E23&amp;","&amp;E24&amp;","&amp;E25&amp;","&amp;E26&amp;"]"</f>
+        <v>[0,1,1,2,1,2,1,1,2,2,1,3,3,2,1,2,3,3,2,1,2,2,1,1,1,1]</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>